<commit_message>
Updated Xcel with current work progress
</commit_message>
<xml_diff>
--- a/Excel sheets/TimeTable Goals.xlsx
+++ b/Excel sheets/TimeTable Goals.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VLAD\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VLAD\Desktop\Github\semester-project-2-\Excel sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBC110E2-1287-4BC9-BFFE-7F61F23D89D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC0E216-BC1D-4807-9399-7BF25004F69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{613330D8-DC9A-4EAB-87C1-FD4A0FB8E11D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="50">
   <si>
     <t>Time</t>
   </si>
@@ -243,6 +243,54 @@
   </si>
   <si>
     <t>NX model of all components</t>
+  </si>
+  <si>
+    <t>New pressure tank succesful up to 150 PSI</t>
+  </si>
+  <si>
+    <t>Testing with water for next time</t>
+  </si>
+  <si>
+    <t>Still waiting on the metal container</t>
+  </si>
+  <si>
+    <t>Waiting for materials</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>Electrical Pump</t>
+    </r>
+  </si>
+  <si>
+    <t>Wrote state changing code</t>
+  </si>
+  <si>
+    <t>To be tested during meeting on the screen</t>
+  </si>
+  <si>
+    <t>Soldering the wires and testing distance of new electric pump</t>
+  </si>
+  <si>
+    <t>During the meeting</t>
   </si>
 </sst>
 </file>
@@ -299,7 +347,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -342,6 +390,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -378,8 +432,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -401,10 +455,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -724,10 +774,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7649D976-40B1-4004-A036-0F04AEBABA71}">
-  <dimension ref="B3:J35"/>
+  <dimension ref="B3:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -880,13 +930,13 @@
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="J18" s="10">
+      <c r="J18" s="11">
         <v>45734</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="8"/>
-      <c r="J19" s="11" t="s">
+      <c r="J19" s="10" t="s">
         <v>27</v>
       </c>
     </row>
@@ -911,7 +961,7 @@
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="J24" s="11" t="s">
+      <c r="J24" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -936,7 +986,7 @@
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="J29" s="11" t="s">
+      <c r="J29" s="10" t="s">
         <v>36</v>
       </c>
     </row>
@@ -956,7 +1006,7 @@
       </c>
     </row>
     <row r="33" spans="10:10" x14ac:dyDescent="0.3">
-      <c r="J33" s="11" t="s">
+      <c r="J33" s="10" t="s">
         <v>39</v>
       </c>
     </row>
@@ -968,6 +1018,105 @@
     <row r="35" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J35" s="9" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J36" s="11">
+        <v>45741</v>
+      </c>
+    </row>
+    <row r="37" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J37" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J38" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J39" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J40" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="41" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J41" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J42" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J43" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J44" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J45" s="9"/>
+    </row>
+    <row r="46" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J46" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J47" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J48" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="49" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J49" s="9"/>
+    </row>
+    <row r="50" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J50" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J51" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="52" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J52" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J53" s="9"/>
+    </row>
+    <row r="54" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J54" s="10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J55" s="9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J56" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -985,6 +1134,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100412B82B521B0A04C828AEAC0B1A91A9B" ma:contentTypeVersion="6" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="ebad0598b07d3e3e10ac38b323e2d045">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="233c9851-1c0e-4fdd-a876-c803d9629353" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01e6cdc39dfb0ba839ee75e2ea541831" ns3:_="">
     <xsd:import namespace="233c9851-1c0e-4fdd-a876-c803d9629353"/>
@@ -1140,15 +1298,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E75065D-CD31-4BE7-BDE4-F2A3AB504F2B}">
   <ds:schemaRefs>
@@ -1166,6 +1315,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{125C4767-9AAC-4736-A8E5-84D14188BE49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{409506E5-A32A-4377-B765-305C841DF2F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1181,12 +1338,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{125C4767-9AAC-4736-A8E5-84D14188BE49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated time table and tasks
</commit_message>
<xml_diff>
--- a/Excel sheets/TimeTable Goals.xlsx
+++ b/Excel sheets/TimeTable Goals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VLAD\Desktop\Github\semester-project-2-\Excel sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952C9803-08FD-41A8-9E5A-FE78760A02EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6778C94B-EFA4-4C2E-83D6-4D41752C81B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{613330D8-DC9A-4EAB-87C1-FD4A0FB8E11D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="90">
   <si>
     <t>Time</t>
   </si>
@@ -382,12 +382,60 @@
   <si>
     <t>Test succeded</t>
   </si>
+  <si>
+    <t>* Radu</t>
+  </si>
+  <si>
+    <t>* Tolga</t>
+  </si>
+  <si>
+    <t>Design x axis</t>
+  </si>
+  <si>
+    <t>encoder holder for x axis</t>
+  </si>
+  <si>
+    <t>* Nikkita</t>
+  </si>
+  <si>
+    <t>Test y axis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Tobias </t>
+  </si>
+  <si>
+    <t>Battery saftey</t>
+  </si>
+  <si>
+    <t>Nothing yet</t>
+  </si>
+  <si>
+    <t>* Mandvias</t>
+  </si>
+  <si>
+    <t>Code for equation in C</t>
+  </si>
+  <si>
+    <t>Battery Bus (Electrical Suply Hub)</t>
+  </si>
+  <si>
+    <t>Translated formula into a function is C code (during meeting)</t>
+  </si>
+  <si>
+    <t>Designing a holder for the motor (during meeting)</t>
+  </si>
+  <si>
+    <t>nothin'</t>
+  </si>
+  <si>
+    <t>·        Electrical Pump</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,6 +496,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Shruti"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -522,7 +576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -538,6 +592,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="4" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -878,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7649D976-40B1-4004-A036-0F04AEBABA71}">
-  <dimension ref="B3:J143"/>
+  <dimension ref="B3:J178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="J128" sqref="J128"/>
+    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
+      <selection activeCell="J179" sqref="J179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1613,6 +1668,142 @@
     <row r="143" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J143" s="9"/>
     </row>
+    <row r="144" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J144" s="11">
+        <v>45789</v>
+      </c>
+    </row>
+    <row r="145" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J145" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="146" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J146" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="147" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J147" s="9"/>
+    </row>
+    <row r="148" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J148" s="9"/>
+    </row>
+    <row r="149" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J149" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="150" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J150" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="151" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J151" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="152" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J152" s="9"/>
+    </row>
+    <row r="153" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J153" s="9"/>
+    </row>
+    <row r="154" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J154" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="155" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J155" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="156" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J156" s="9"/>
+    </row>
+    <row r="157" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J157" s="9"/>
+    </row>
+    <row r="158" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J158" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="159" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J159" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="160" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J160" s="9"/>
+    </row>
+    <row r="161" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J161" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="162" spans="10:10" ht="18.600000000000001" x14ac:dyDescent="0.6">
+      <c r="J162" s="13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="164" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J164" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="165" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J165" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="167" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J167" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="168" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J168" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="169" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J169" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="171" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J171" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="172" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J172" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="174" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J174" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="175" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J175" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="177" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J177" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="178" spans="10:10" x14ac:dyDescent="0.3">
+      <c r="J178" t="s">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1621,23 +1812,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="233c9851-1c0e-4fdd-a876-c803d9629353" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100412B82B521B0A04C828AEAC0B1A91A9B" ma:contentTypeVersion="6" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="ebad0598b07d3e3e10ac38b323e2d045">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="233c9851-1c0e-4fdd-a876-c803d9629353" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="01e6cdc39dfb0ba839ee75e2ea541831" ns3:_="">
     <xsd:import namespace="233c9851-1c0e-4fdd-a876-c803d9629353"/>
@@ -1793,31 +1967,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E75065D-CD31-4BE7-BDE4-F2A3AB504F2B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="233c9851-1c0e-4fdd-a876-c803d9629353"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{125C4767-9AAC-4736-A8E5-84D14188BE49}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="233c9851-1c0e-4fdd-a876-c803d9629353" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{409506E5-A32A-4377-B765-305C841DF2F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1833,4 +2000,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{125C4767-9AAC-4736-A8E5-84D14188BE49}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E75065D-CD31-4BE7-BDE4-F2A3AB504F2B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="233c9851-1c0e-4fdd-a876-c803d9629353"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>